<commit_message>
Update Rizka - Tambah Akun Bank v2 Excel
</commit_message>
<xml_diff>
--- a/TambahAkunBank.xlsx
+++ b/TambahAkunBank.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marvin\Documents\GitHub\ACC-Seamless\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A736D0-53F7-4495-95E3-F5D5406E7CFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22839BA-FF37-4E7C-B80A-DECE3F1E0C04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1537C384-1F8A-4666-B5E5-0A13BA97C185}"/>
+    <workbookView xWindow="390" yWindow="0" windowWidth="13440" windowHeight="11070" activeTab="1" xr2:uid="{1537C384-1F8A-4666-B5E5-0A13BA97C185}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v1" sheetId="1" r:id="rId1"/>
+    <sheet name="v2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>NamaBank</t>
   </si>
@@ -39,9 +40,6 @@
     <t>Cabang</t>
   </si>
   <si>
-    <t>KataSandi</t>
-  </si>
-  <si>
     <t>OTP</t>
   </si>
   <si>
@@ -60,9 +58,6 @@
     <t>Tony Stark</t>
   </si>
   <si>
-    <t>Johannes!12</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -108,9 +103,6 @@
     <t>Bucky Barners</t>
   </si>
   <si>
-    <t>Johannes</t>
-  </si>
-  <si>
     <t>Password Salah</t>
   </si>
   <si>
@@ -124,13 +116,79 @@
   </si>
   <si>
     <t>NoRek</t>
+  </si>
+  <si>
+    <t>namaBank</t>
+  </si>
+  <si>
+    <t>cabang</t>
+  </si>
+  <si>
+    <t>namaPemilikRek</t>
+  </si>
+  <si>
+    <t>noRek</t>
+  </si>
+  <si>
+    <t>jadikanUtama</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>MANDIRI-SMD-MULAWARMAN</t>
+  </si>
+  <si>
+    <t>Rizka</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>dropDownKosong</t>
+  </si>
+  <si>
+    <t>noRekMin8Angka</t>
+  </si>
+  <si>
+    <t>namaMin3Huruf</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Panda</t>
+  </si>
+  <si>
+    <t>Adjie</t>
+  </si>
+  <si>
+    <t>noRekTidakBolehSama</t>
+  </si>
+  <si>
+    <t>Denna</t>
+  </si>
+  <si>
+    <t>OTPsalah</t>
+  </si>
+  <si>
+    <t>backButton</t>
+  </si>
+  <si>
+    <t>Az</t>
+  </si>
+  <si>
+    <t>Alda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,16 +196,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -155,12 +239,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BAABA3-1D04-4F43-9F6D-7729D1EF9E54}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,235 +610,438 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>333563612</v>
+      </c>
+      <c r="E2">
+        <v>261294</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>333563612</v>
+      </c>
+      <c r="E3">
+        <v>261294</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>333563616</v>
+      </c>
+      <c r="E4">
+        <v>261294</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>333563616</v>
+      </c>
+      <c r="E5">
+        <v>261294</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>261294</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>333563616</v>
+      </c>
+      <c r="E7">
+        <v>261294</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>333563616</v>
+      </c>
+      <c r="E8">
+        <v>261294</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>333563616</v>
+      </c>
+      <c r="E9">
+        <v>234234</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DF0AFA-565D-434E-918B-5A0E5A5CA65C}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
+      <c r="G1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>333563612</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="3">
         <v>261294</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
+      <c r="G2" s="10"/>
+      <c r="H2" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>333563612</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4">
+        <v>12345678</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5">
         <v>261294</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
+      <c r="G3" s="10"/>
+      <c r="H3" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>333563616</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="4">
+        <v>12345678</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="5">
         <v>261294</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>333563616</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5">
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="7">
+        <v>12345</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="5">
         <v>261294</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
+      <c r="G5" s="10"/>
+      <c r="H5" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>261294</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="7">
+        <v>11111111</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="5">
+        <v>261295</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7">
-        <v>333563616</v>
-      </c>
-      <c r="F7">
-        <v>261294</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="4">
+        <v>12345680</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="6">
+        <v>444444</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8">
-        <v>333563616</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8">
-        <v>261294</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>26</v>
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9">
-        <v>333563616</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>234234</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>